<commit_message>
made all phrases into single word for card.json
</commit_message>
<xml_diff>
--- a/src/Data/translated_phrases.xlsx
+++ b/src/Data/translated_phrases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davide/Projects/week16/react-flashcards/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD160EC-9DFA-274A-9ECF-611A4D763705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C0469A-B82A-EB47-962F-81AE776128D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="34400" windowHeight="26740" activeTab="2" xr2:uid="{C54B77F0-B43A-1646-AF32-4C919672BDFB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="26740" xr2:uid="{C54B77F0-B43A-1646-AF32-4C919672BDFB}"/>
   </bookViews>
   <sheets>
     <sheet name="russian" sheetId="3" r:id="rId1"/>
@@ -32,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
-  <si>
-    <t>I have a question</t>
-  </si>
-  <si>
-    <t>I have a sister</t>
-  </si>
-  <si>
-    <t>У меня есть сестра</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>english</t>
   </si>
@@ -49,9 +40,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>to have</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -82,31 +70,58 @@
     <t>Fàguó</t>
   </si>
   <si>
-    <t>У меня есть вопрос</t>
-  </si>
-  <si>
-    <t>u menya est vopros</t>
-  </si>
-  <si>
-    <t>u menya est sestra</t>
-  </si>
-  <si>
-    <t>Dov'è la toilette</t>
-  </si>
-  <si>
     <t>toilet directions</t>
   </si>
   <si>
-    <t>grazie per l'informazione</t>
-  </si>
-  <si>
-    <t>Where is the toilet?</t>
-  </si>
-  <si>
-    <t>Thanks for the information</t>
-  </si>
-  <si>
     <t>pleasantries</t>
+  </si>
+  <si>
+    <t>toilette</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>informazione</t>
+  </si>
+  <si>
+    <t>information</t>
+  </si>
+  <si>
+    <t>grazie</t>
+  </si>
+  <si>
+    <t>thank you</t>
+  </si>
+  <si>
+    <t>вопрос</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>vopros</t>
+  </si>
+  <si>
+    <t>сестра</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>sister</t>
+  </si>
+  <si>
+    <t>sestra</t>
+  </si>
+  <si>
+    <t>брат</t>
+  </si>
+  <si>
+    <t>brother</t>
+  </si>
+  <si>
+    <t>brat</t>
   </si>
 </sst>
 </file>
@@ -461,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBE5071-1CE1-D24D-8A1B-2EEB9FB8F7CA}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,48 +493,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -531,7 +560,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,46 +573,46 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -594,10 +623,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC0E75B-6583-EB46-9D42-CCB3FCCC67A1}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,42 +639,53 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moved database opening to flashCardPage
</commit_message>
<xml_diff>
--- a/src/Data/translated_phrases.xlsx
+++ b/src/Data/translated_phrases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davide/Projects/week16/react-flashcards/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C0469A-B82A-EB47-962F-81AE776128D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE80829-3737-394F-9C29-31204D8B5DA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="26740" xr2:uid="{C54B77F0-B43A-1646-AF32-4C919672BDFB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38660" windowHeight="26740" xr2:uid="{C54B77F0-B43A-1646-AF32-4C919672BDFB}"/>
   </bookViews>
   <sheets>
     <sheet name="russian" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
   <si>
     <t>english</t>
   </si>
@@ -122,6 +122,273 @@
   </si>
   <si>
     <t>brat</t>
+  </si>
+  <si>
+    <t>привет</t>
+  </si>
+  <si>
+    <t>greeting</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>preevyet</t>
+  </si>
+  <si>
+    <t>кот</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>kot</t>
+  </si>
+  <si>
+    <t>собака</t>
+  </si>
+  <si>
+    <t>слон</t>
+  </si>
+  <si>
+    <t>жираф</t>
+  </si>
+  <si>
+    <t>дельфин</t>
+  </si>
+  <si>
+    <t>заяц</t>
+  </si>
+  <si>
+    <t>енот</t>
+  </si>
+  <si>
+    <t>змея</t>
+  </si>
+  <si>
+    <t>волк</t>
+  </si>
+  <si>
+    <t>лиса</t>
+  </si>
+  <si>
+    <t>белка</t>
+  </si>
+  <si>
+    <t>птица</t>
+  </si>
+  <si>
+    <t>рыба</t>
+  </si>
+  <si>
+    <t>девушка</t>
+  </si>
+  <si>
+    <t>женщина</t>
+  </si>
+  <si>
+    <t>мужчина</t>
+  </si>
+  <si>
+    <t>ребёнок</t>
+  </si>
+  <si>
+    <t>ёж</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>sabaka</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>slon</t>
+  </si>
+  <si>
+    <t>giraffe</t>
+  </si>
+  <si>
+    <t>zheraf</t>
+  </si>
+  <si>
+    <t>dolphin</t>
+  </si>
+  <si>
+    <t>delfeen</t>
+  </si>
+  <si>
+    <t>hare</t>
+  </si>
+  <si>
+    <t>zayats</t>
+  </si>
+  <si>
+    <t>racoon</t>
+  </si>
+  <si>
+    <t>yenot</t>
+  </si>
+  <si>
+    <t>snake</t>
+  </si>
+  <si>
+    <t>zmeya</t>
+  </si>
+  <si>
+    <t>wolf</t>
+  </si>
+  <si>
+    <t>volk</t>
+  </si>
+  <si>
+    <t>fox</t>
+  </si>
+  <si>
+    <t>leysa</t>
+  </si>
+  <si>
+    <t>squirrel</t>
+  </si>
+  <si>
+    <t>vyelka</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>pteetsa</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>reeba</t>
+  </si>
+  <si>
+    <t>girl</t>
+  </si>
+  <si>
+    <t>dyevyshka</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t>zhensheena</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>moosheena</t>
+  </si>
+  <si>
+    <t>kid</t>
+  </si>
+  <si>
+    <t>rebyonak</t>
+  </si>
+  <si>
+    <t>hedgehog</t>
+  </si>
+  <si>
+    <t>yozh</t>
+  </si>
+  <si>
+    <t>медведь</t>
+  </si>
+  <si>
+    <t>девочка</t>
+  </si>
+  <si>
+    <t>мальчик</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>bear</t>
+  </si>
+  <si>
+    <t>medvedt</t>
+  </si>
+  <si>
+    <t>devochka</t>
+  </si>
+  <si>
+    <t>boy</t>
+  </si>
+  <si>
+    <t>malcheek</t>
+  </si>
+  <si>
+    <t>бабушка</t>
+  </si>
+  <si>
+    <t>дедушка</t>
+  </si>
+  <si>
+    <t>мама</t>
+  </si>
+  <si>
+    <t>папа</t>
+  </si>
+  <si>
+    <t>семья</t>
+  </si>
+  <si>
+    <t>dad</t>
+  </si>
+  <si>
+    <t>mum</t>
+  </si>
+  <si>
+    <t>grandfather</t>
+  </si>
+  <si>
+    <t>grandmother</t>
+  </si>
+  <si>
+    <t>babooshka</t>
+  </si>
+  <si>
+    <t>dyedooshka</t>
+  </si>
+  <si>
+    <t>mama</t>
+  </si>
+  <si>
+    <t>papa</t>
+  </si>
+  <si>
+    <t>semya</t>
+  </si>
+  <si>
+    <t>мой/моя</t>
+  </si>
+  <si>
+    <t>твой/твоя</t>
+  </si>
+  <si>
+    <t>preposition</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>moy/maya</t>
+  </si>
+  <si>
+    <t>your</t>
+  </si>
+  <si>
+    <t>tvoy/tvaya</t>
   </si>
 </sst>
 </file>
@@ -157,10 +424,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBE5071-1CE1-D24D-8A1B-2EEB9FB8F7CA}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,6 +819,416 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>